<commit_message>
Added stats nmt 8
</commit_message>
<xml_diff>
--- a/nmt/stats/nmt_score.xlsx
+++ b/nmt/stats/nmt_score.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t xml:space="preserve">Scoring File Name</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t xml:space="preserve">Nmt_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nmt_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_186k+case</t>
   </si>
 </sst>
 </file>
@@ -269,13 +275,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
@@ -427,6 +433,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>